<commit_message>
full working everything (still need to implement queues and EH)... Working on deploying to orchestrator
</commit_message>
<xml_diff>
--- a/HansenBeauProject2/Accessory Files/Orders2.xlsx
+++ b/HansenBeauProject2/Accessory Files/Orders2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\revature\Uipath Processes\ProjectTwoRepository\HansenBeauProject2\Accessory Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04BA1516-66EB-4468-875F-37D7BA815518}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE1735BD-3E6B-4D80-A244-7B52B925C1E1}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8988" activeTab="1" xr2:uid="{4BDC7A61-A714-42CE-B3C7-8A0E9755D3A4}"/>
   </bookViews>
@@ -125,7 +125,7 @@
     <t>Successful</t>
   </si>
   <si>
-    <t>Order #512574</t>
+    <t>Order #512626</t>
   </si>
 </sst>
 </file>
@@ -583,7 +583,7 @@
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Everything invoked... queues implemented... deployed to orchestrator
</commit_message>
<xml_diff>
--- a/HansenBeauProject2/Accessory Files/Orders2.xlsx
+++ b/HansenBeauProject2/Accessory Files/Orders2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\revature\Uipath Processes\ProjectTwoRepository\HansenBeauProject2\Accessory Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B59565B-791D-446E-ABBF-F01CDD31027F}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FADF8208-3D6C-45BC-B25D-09A094F81367}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8988" activeTab="1" xr2:uid="{4BDC7A61-A714-42CE-B3C7-8A0E9755D3A4}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="35">
   <si>
     <t>Product</t>
   </si>
@@ -137,10 +137,7 @@
     <t>MicroSoft</t>
   </si>
   <si>
-    <t>Item is out of stock (zero value). Order was not placed</t>
-  </si>
-  <si>
-    <t>Order #512695</t>
+    <t>Order #512711</t>
   </si>
 </sst>
 </file>
@@ -598,7 +595,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32EA5CF3-CE25-4BAD-A587-40126C152148}">
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
@@ -613,7 +610,7 @@
     <col min="6" max="6" width="9.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -633,7 +630,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -644,7 +641,7 @@
         <v>28</v>
       </c>
       <c r="D2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E2" s="1">
         <v>10</v>
@@ -652,8 +649,11 @@
       <c r="F2" s="1">
         <v>20</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H2" s="1">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -661,15 +661,19 @@
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="D3" t="s">
         <v>34</v>
       </c>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E3" s="1">
+        <v>23</v>
+      </c>
+      <c r="F3" s="1">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -680,7 +684,7 @@
         <v>28</v>
       </c>
       <c r="D4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E4" s="1">
         <v>7</v>
@@ -689,7 +693,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -700,7 +704,7 @@
         <v>28</v>
       </c>
       <c r="D5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E5" s="1">
         <v>7.5</v>
@@ -709,7 +713,7 @@
         <v>7.5</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -720,7 +724,7 @@
         <v>28</v>
       </c>
       <c r="D6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E6" s="1">
         <v>2.25</v>
@@ -729,7 +733,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -740,7 +744,7 @@
         <v>28</v>
       </c>
       <c r="D7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E7" s="1">
         <v>9</v>
@@ -749,7 +753,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -760,7 +764,7 @@
         <v>28</v>
       </c>
       <c r="D8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E8" s="1">
         <v>7</v>
@@ -769,7 +773,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -783,39 +787,19 @@
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C10" t="s">
-        <v>28</v>
-      </c>
-      <c r="D10" t="s">
-        <v>35</v>
-      </c>
-      <c r="E10" s="1">
-        <v>7</v>
-      </c>
-      <c r="F10" s="1">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C11" t="s">
-        <v>28</v>
-      </c>
-      <c r="D11" t="s">
-        <v>35</v>
-      </c>
-      <c r="E11" s="1">
-        <v>7</v>
-      </c>
-      <c r="F11" s="1">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
     </row>

</xml_diff>